<commit_message>
Main Assignment TC02-Add 3 items to cart
</commit_message>
<xml_diff>
--- a/Main_Sel_Assignment/Utils/Assignment.xlsx
+++ b/Main_Sel_Assignment/Utils/Assignment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vbalasubramaniyam/Documents/GitHub/HuTraining/Main_Sel_Assignment/Utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4931BD3-71C6-F44F-996B-201072263D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C2C17D-AC7D-D347-91FD-860FF4915DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{6423E178-F58C-F64F-A78F-C0B6757F79EF}"/>
+    <workbookView xWindow="1480" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{6423E178-F58C-F64F-A78F-C0B6757F79EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>99952622682</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Password</t>
   </si>
@@ -57,20 +54,50 @@
     <t>TestCase3</t>
   </si>
   <si>
-    <t>vino@124</t>
-  </si>
-  <si>
-    <t>vino@125</t>
-  </si>
-  <si>
     <t>Vino@123</t>
+  </si>
+  <si>
+    <t>9952622682</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>Sunfeast Dark Fantasy Choco Fills Cream Filled</t>
+  </si>
+  <si>
+    <t>Product2</t>
+  </si>
+  <si>
+    <t>Parrys White Label Sugar</t>
+  </si>
+  <si>
+    <t>Product3</t>
+  </si>
+  <si>
+    <t>PARLE Wafers Cream and Onion</t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>641402</t>
+  </si>
+  <si>
+    <t>Bingo Mad Angles Achaari Masti Chips Chips</t>
+  </si>
+  <si>
+    <t>Parry's White Label Sugar</t>
+  </si>
+  <si>
+    <t>product2_dub</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +115,19 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,10 +154,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -433,67 +475,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E5CD55-E1C1-F648-AE18-5086CF0C9402}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="vino@123" xr:uid="{B8A0DC05-CADA-944C-90D5-0985DCDF635F}"/>
-    <hyperlink ref="C3:C4" r:id="rId2" display="vino@123" xr:uid="{0BCAA620-664E-E948-BD84-88648196A5EC}"/>
+    <hyperlink ref="C3" r:id="rId2" display="vino@123" xr:uid="{17918D95-38C7-1A4F-8ABA-5F5ECB9B50BD}"/>
+    <hyperlink ref="C4" r:id="rId3" display="vino@123" xr:uid="{7323CFD2-030F-AC44-989A-7DE8991E0F3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Main Assignment TC04-Add Profile Address
</commit_message>
<xml_diff>
--- a/Main_Sel_Assignment/Utils/Assignment.xlsx
+++ b/Main_Sel_Assignment/Utils/Assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vbalasubramaniyam/Documents/GitHub/HuTraining/Main_Sel_Assignment/Utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C2C17D-AC7D-D347-91FD-860FF4915DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02D270E-7065-454E-979B-FCDBEA7AB51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{6423E178-F58C-F64F-A78F-C0B6757F79EF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Password</t>
   </si>
@@ -91,6 +91,36 @@
   </si>
   <si>
     <t>product2_dub</t>
+  </si>
+  <si>
+    <t>TestCase4</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>flocality</t>
+  </si>
+  <si>
+    <t>faddress</t>
+  </si>
+  <si>
+    <t>fcity</t>
+  </si>
+  <si>
+    <t>fstate</t>
+  </si>
+  <si>
+    <t>Vino</t>
+  </si>
+  <si>
+    <t>coimbatore</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>airforce station,sulur</t>
   </si>
 </sst>
 </file>
@@ -475,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E5CD55-E1C1-F648-AE18-5086CF0C9402}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -489,7 +519,7 @@
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -514,8 +544,23 @@
       <c r="H1" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -541,7 +586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -567,7 +612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -576,6 +621,62 @@
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -584,6 +685,7 @@
     <hyperlink ref="C2" r:id="rId1" display="vino@123" xr:uid="{B8A0DC05-CADA-944C-90D5-0985DCDF635F}"/>
     <hyperlink ref="C3" r:id="rId2" display="vino@123" xr:uid="{17918D95-38C7-1A4F-8ABA-5F5ECB9B50BD}"/>
     <hyperlink ref="C4" r:id="rId3" display="vino@123" xr:uid="{7323CFD2-030F-AC44-989A-7DE8991E0F3F}"/>
+    <hyperlink ref="C5" r:id="rId4" display="vino@123" xr:uid="{34A581F4-94C4-204C-B3C7-AAC5530DA32B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Comments added to the methods
</commit_message>
<xml_diff>
--- a/Main_Sel_Assignment/Utils/Assignment.xlsx
+++ b/Main_Sel_Assignment/Utils/Assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vbalasubramaniyam/Documents/GitHub/HuTraining/Main_Sel_Assignment/Utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D6627E-D6AB-8B47-98C0-5D124456E8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5079B129-ADDD-3141-9A80-BA6ECD032DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{6423E178-F58C-F64F-A78F-C0B6757F79EF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>Password</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>airforce station,sulur</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>TATA</t>
   </si>
 </sst>
 </file>
@@ -505,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E5CD55-E1C1-F648-AE18-5086CF0C9402}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -519,7 +525,7 @@
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -559,8 +565,11 @@
       <c r="M1" t="s">
         <v>24</v>
       </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -585,8 +594,11 @@
       <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -611,8 +623,11 @@
       <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -637,8 +652,11 @@
       <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Updated Search and Filter tc
</commit_message>
<xml_diff>
--- a/Main_Sel_Assignment/Utils/Assignment.xlsx
+++ b/Main_Sel_Assignment/Utils/Assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vbalasubramaniyam/Documents/GitHub/HuTraining/Main_Sel_Assignment/Utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5079B129-ADDD-3141-9A80-BA6ECD032DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C37BC9-1EFC-C247-81BC-B5912AB2A45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{6423E178-F58C-F64F-A78F-C0B6757F79EF}"/>
   </bookViews>
@@ -126,7 +126,7 @@
     <t>brand</t>
   </si>
   <si>
-    <t>TATA</t>
+    <t>Tata</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="N2" sqref="N2:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>